<commit_message>
Updating mutsig and oncoplot scripts
</commit_message>
<xml_diff>
--- a/cosmic/COSMIC_signature_etiology.xlsx
+++ b/cosmic/COSMIC_signature_etiology.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tandonm/Documents/ccbr1051_simon/5/data/cosmic/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tandonm/Documents/helper_functions/git_repo/mt_helpers/cosmic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A07A757-0A8F-A640-9B16-C6BF8DCF078D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFAC704-0FEF-1B42-8352-BEE3F6074C24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="3560" windowWidth="27640" windowHeight="16940" xr2:uid="{C8441BA4-CE16-794D-B8BF-FAC856A78B1B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SBS" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -2614,7 +2614,7 @@
         <v>174</v>
       </c>
       <c r="B2">
-        <f>COUNTIF(Sheet1!$B$2:$B$73,Sheet2!A2)</f>
+        <f>COUNTIF(SBS!$B$2:$B$73,Sheet2!A2)</f>
         <v>12</v>
       </c>
       <c r="C2" s="2">
@@ -2627,7 +2627,7 @@
         <v>175</v>
       </c>
       <c r="B3">
-        <f>COUNTIF(Sheet1!$B$2:$B$73,Sheet2!A3)</f>
+        <f>COUNTIF(SBS!$B$2:$B$73,Sheet2!A3)</f>
         <v>3</v>
       </c>
       <c r="C3" s="2">
@@ -2640,7 +2640,7 @@
         <v>173</v>
       </c>
       <c r="B4">
-        <f>COUNTIF(Sheet1!$B$2:$B$73,Sheet2!A4)</f>
+        <f>COUNTIF(SBS!$B$2:$B$73,Sheet2!A4)</f>
         <v>4</v>
       </c>
       <c r="C4" s="2">
@@ -2653,7 +2653,7 @@
         <v>170</v>
       </c>
       <c r="B5">
-        <f>COUNTIF(Sheet1!$B$2:$B$73,Sheet2!A5)</f>
+        <f>COUNTIF(SBS!$B$2:$B$73,Sheet2!A5)</f>
         <v>15</v>
       </c>
       <c r="C5" s="2">
@@ -2666,7 +2666,7 @@
         <v>171</v>
       </c>
       <c r="B6">
-        <f>COUNTIF(Sheet1!$B$2:$B$73,Sheet2!A6)</f>
+        <f>COUNTIF(SBS!$B$2:$B$73,Sheet2!A6)</f>
         <v>0</v>
       </c>
       <c r="C6" s="2">
@@ -2679,7 +2679,7 @@
         <v>176</v>
       </c>
       <c r="B7">
-        <f>COUNTIF(Sheet1!$B$2:$B$73,Sheet2!A7)</f>
+        <f>COUNTIF(SBS!$B$2:$B$73,Sheet2!A7)</f>
         <v>3</v>
       </c>
       <c r="C7" s="2">
@@ -2692,7 +2692,7 @@
         <v>177</v>
       </c>
       <c r="B8">
-        <f>COUNTIF(Sheet1!$B$2:$B$73,Sheet2!A8)</f>
+        <f>COUNTIF(SBS!$B$2:$B$73,Sheet2!A8)</f>
         <v>7</v>
       </c>
       <c r="C8" s="2">
@@ -2705,7 +2705,7 @@
         <v>178</v>
       </c>
       <c r="B9">
-        <f>COUNTIF(Sheet1!$B$2:$B$73,Sheet2!A9)</f>
+        <f>COUNTIF(SBS!$B$2:$B$73,Sheet2!A9)</f>
         <v>1</v>
       </c>
       <c r="C9" s="2">
@@ -2718,7 +2718,7 @@
         <v>180</v>
       </c>
       <c r="B10">
-        <f>COUNTIF(Sheet1!$B$2:$B$73,Sheet2!A10)</f>
+        <f>COUNTIF(SBS!$B$2:$B$73,Sheet2!A10)</f>
         <v>4</v>
       </c>
       <c r="C10" s="2">
@@ -2731,7 +2731,7 @@
         <v>181</v>
       </c>
       <c r="B11">
-        <f>COUNTIF(Sheet1!$B$2:$B$73,Sheet2!A11)</f>
+        <f>COUNTIF(SBS!$B$2:$B$73,Sheet2!A11)</f>
         <v>18</v>
       </c>
       <c r="C11" s="2">
@@ -2750,7 +2750,7 @@
         <v>192</v>
       </c>
       <c r="B16">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A16)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A16)</f>
         <v>1</v>
       </c>
       <c r="C16" s="2">
@@ -2763,7 +2763,7 @@
         <v>169</v>
       </c>
       <c r="B17">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A17)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A17)</f>
         <v>0</v>
       </c>
       <c r="C17" s="2">
@@ -2776,7 +2776,7 @@
         <v>164</v>
       </c>
       <c r="B18">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A18)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A18)</f>
         <v>2</v>
       </c>
       <c r="C18" s="2">
@@ -2789,7 +2789,7 @@
         <v>201</v>
       </c>
       <c r="B19">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A19)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A19)</f>
         <v>0</v>
       </c>
       <c r="C19" s="2">
@@ -2802,7 +2802,7 @@
         <v>193</v>
       </c>
       <c r="B20">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A20)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A20)</f>
         <v>1</v>
       </c>
       <c r="C20" s="2">
@@ -2815,7 +2815,7 @@
         <v>194</v>
       </c>
       <c r="B21">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A21)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A21)</f>
         <v>1</v>
       </c>
       <c r="C21" s="2">
@@ -2828,7 +2828,7 @@
         <v>195</v>
       </c>
       <c r="B22">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A22)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A22)</f>
         <v>1</v>
       </c>
       <c r="C22" s="2">
@@ -2841,7 +2841,7 @@
         <v>196</v>
       </c>
       <c r="B23">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A23)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A23)</f>
         <v>1</v>
       </c>
       <c r="C23" s="2">
@@ -2854,7 +2854,7 @@
         <v>197</v>
       </c>
       <c r="B24">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A24)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A24)</f>
         <v>7</v>
       </c>
       <c r="C24" s="2">
@@ -2867,7 +2867,7 @@
         <v>199</v>
       </c>
       <c r="B25">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A25)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A25)</f>
         <v>0</v>
       </c>
       <c r="C25" s="2">
@@ -2880,7 +2880,7 @@
         <v>171</v>
       </c>
       <c r="B26">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A26)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A26)</f>
         <v>4</v>
       </c>
       <c r="C26" s="2">
@@ -2893,7 +2893,7 @@
         <v>170</v>
       </c>
       <c r="B27">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A27)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A27)</f>
         <v>13</v>
       </c>
       <c r="C27" s="2">
@@ -2906,7 +2906,7 @@
         <v>200</v>
       </c>
       <c r="B28">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A28)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A28)</f>
         <v>1</v>
       </c>
       <c r="C28" s="2">
@@ -2919,7 +2919,7 @@
         <v>166</v>
       </c>
       <c r="B29">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A29)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A29)</f>
         <v>0</v>
       </c>
       <c r="C29" s="2">
@@ -2932,7 +2932,7 @@
         <v>167</v>
       </c>
       <c r="B30">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A30)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A30)</f>
         <v>0</v>
       </c>
       <c r="C30" s="2">
@@ -2945,7 +2945,7 @@
         <v>179</v>
       </c>
       <c r="B31">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A31)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A31)</f>
         <v>0</v>
       </c>
       <c r="C31" s="2">
@@ -2958,7 +2958,7 @@
         <v>165</v>
       </c>
       <c r="B32">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A32)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A32)</f>
         <v>0</v>
       </c>
       <c r="C32" s="2">
@@ -2971,7 +2971,7 @@
         <v>182</v>
       </c>
       <c r="B33">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A33)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A33)</f>
         <v>14</v>
       </c>
       <c r="C33" s="2">
@@ -2984,7 +2984,7 @@
         <v>183</v>
       </c>
       <c r="B34">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A34)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A34)</f>
         <v>2</v>
       </c>
       <c r="C34" s="2">
@@ -2997,7 +2997,7 @@
         <v>184</v>
       </c>
       <c r="B35">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A35)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A35)</f>
         <v>2</v>
       </c>
       <c r="C35" s="2">
@@ -3010,7 +3010,7 @@
         <v>185</v>
       </c>
       <c r="B36">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A36)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A36)</f>
         <v>0</v>
       </c>
       <c r="C36" s="2">
@@ -3023,7 +3023,7 @@
         <v>186</v>
       </c>
       <c r="B37">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A37)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A37)</f>
         <v>0</v>
       </c>
       <c r="C37" s="2">
@@ -3036,7 +3036,7 @@
         <v>187</v>
       </c>
       <c r="B38">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A38)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A38)</f>
         <v>0</v>
       </c>
       <c r="C38" s="2">
@@ -3049,7 +3049,7 @@
         <v>188</v>
       </c>
       <c r="B39">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A39)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A39)</f>
         <v>0</v>
       </c>
       <c r="C39" s="2">
@@ -3062,7 +3062,7 @@
         <v>189</v>
       </c>
       <c r="B40">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A40)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A40)</f>
         <v>0</v>
       </c>
       <c r="C40" s="2">
@@ -3075,7 +3075,7 @@
         <v>168</v>
       </c>
       <c r="B41">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A41)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A41)</f>
         <v>0</v>
       </c>
       <c r="C41" s="2">
@@ -3088,7 +3088,7 @@
         <v>172</v>
       </c>
       <c r="B42">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A42)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A42)</f>
         <v>1</v>
       </c>
       <c r="C42" s="2">
@@ -3101,7 +3101,7 @@
         <v>190</v>
       </c>
       <c r="B43">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A43)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A43)</f>
         <v>4</v>
       </c>
       <c r="C43" s="2">
@@ -3114,7 +3114,7 @@
         <v>191</v>
       </c>
       <c r="B44">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A44)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A44)</f>
         <v>2</v>
       </c>
       <c r="C44" s="2">
@@ -3127,7 +3127,7 @@
         <v>198</v>
       </c>
       <c r="B45">
-        <f>COUNTIF(Sheet1!$C$2:$C$73,Sheet2!A45)</f>
+        <f>COUNTIF(SBS!$C$2:$C$73,Sheet2!A45)</f>
         <v>1</v>
       </c>
       <c r="C45" s="2">

</xml_diff>